<commit_message>
interupts collection and stuff
</commit_message>
<xml_diff>
--- a/ESP_Output.xlsx
+++ b/ESP_Output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A49"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,336 +443,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>284</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>295</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>322</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>371</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>393</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>416</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>659</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>687</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>713</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>737</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>760</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>9754</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>9781</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>9806</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>9823</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>9831</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>9856</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>9881</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>9905</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>9930</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>9955</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>9980</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>10004</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>10029</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>10054</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>10078</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>10102</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>10127</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>10151</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>10176</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>10201</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>10226</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>10251</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>10277</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>10302</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>10327</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>10352</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>10377</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>10402</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>10426</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>10451</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>10475</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>10499</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>10523</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>10547</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>10571</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>13038</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>-87497</t>
+          <t>-87519</t>
         </is>
       </c>
     </row>

</xml_diff>